<commit_message>
Removes FileList.csv, adds updated LocalFileList.xlsx, and adds various portions to code, including comments.
</commit_message>
<xml_diff>
--- a/LocalFileList.xlsx
+++ b/LocalFileList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\ROneDrive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\fight\Documents\ROneDrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84154073-9CFE-4ABC-85FC-9892AAA3B5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B74FB5-826F-45FF-8CFF-4DFD06B15590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8A96415-ACA3-4E3A-B8C9-9338A28545D5}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{F8A96415-ACA3-4E3A-B8C9-9338A28545D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,28 +49,28 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>D:/My Files/Army Stuff</t>
-  </si>
-  <si>
-    <t>D:/My Files/My Personal Stuff/Coursera Certificates</t>
-  </si>
-  <si>
-    <t>D:/My Files/My Personal Stuff/Marching Band</t>
-  </si>
-  <si>
-    <t>D:/My Files/My Personal Stuff/Red Book and YouTube Video List</t>
-  </si>
-  <si>
-    <t>D:/My Files/My Personal Stuff/Taxes</t>
-  </si>
-  <si>
-    <t>D:/My Files/My Personal Stuff/Warhammer 40K</t>
-  </si>
-  <si>
-    <t>D:/My Files/My Personal Stuff/Wedding</t>
-  </si>
-  <si>
-    <t>D:/My Files/My Personal Stuff</t>
+    <t>F:/My Files/Army Stuff</t>
+  </si>
+  <si>
+    <t>F:/My Files/My Personal Stuff</t>
+  </si>
+  <si>
+    <t>F:/My Files/My Personal Stuff/Coursera Certificates</t>
+  </si>
+  <si>
+    <t>F:/My Files/My Personal Stuff/Marching Band</t>
+  </si>
+  <si>
+    <t>F:/My Files/My Personal Stuff/Red Book and YouTube Video List</t>
+  </si>
+  <si>
+    <t>F:/My Files/My Personal Stuff/Taxes</t>
+  </si>
+  <si>
+    <t>F:/My Files/My Personal Stuff/Warhammer 40K</t>
+  </si>
+  <si>
+    <t>F:/My Files/My Personal Stuff/Wedding</t>
   </si>
 </sst>
 </file>
@@ -434,16 +434,16 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="59.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -451,7 +451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -459,42 +459,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Updated local file list for desktop. -Tested code and it appears to work as intended.
</commit_message>
<xml_diff>
--- a/LocalFileList.xlsx
+++ b/LocalFileList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\fight\Documents\ROneDrive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\ROneDrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B74FB5-826F-45FF-8CFF-4DFD06B15590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15488D5B-778C-42BE-8E59-636932B2A17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{F8A96415-ACA3-4E3A-B8C9-9338A28545D5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8A96415-ACA3-4E3A-B8C9-9338A28545D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,28 +49,28 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>F:/My Files/Army Stuff</t>
-  </si>
-  <si>
-    <t>F:/My Files/My Personal Stuff</t>
-  </si>
-  <si>
-    <t>F:/My Files/My Personal Stuff/Coursera Certificates</t>
-  </si>
-  <si>
-    <t>F:/My Files/My Personal Stuff/Marching Band</t>
-  </si>
-  <si>
-    <t>F:/My Files/My Personal Stuff/Red Book and YouTube Video List</t>
-  </si>
-  <si>
-    <t>F:/My Files/My Personal Stuff/Taxes</t>
-  </si>
-  <si>
-    <t>F:/My Files/My Personal Stuff/Warhammer 40K</t>
-  </si>
-  <si>
-    <t>F:/My Files/My Personal Stuff/Wedding</t>
+    <t>D:/My Files/Army Stuff</t>
+  </si>
+  <si>
+    <t>D:/My Files/My Personal Stuff</t>
+  </si>
+  <si>
+    <t>D:/My Files/My Personal Stuff/Coursera Certificates</t>
+  </si>
+  <si>
+    <t>D:/My Files/My Personal Stuff/Marching Band</t>
+  </si>
+  <si>
+    <t>D:/My Files/My Personal Stuff/Red Book and YouTube Video List</t>
+  </si>
+  <si>
+    <t>D:/My Files/My Personal Stuff/Taxes</t>
+  </si>
+  <si>
+    <t>D:/My Files/My Personal Stuff/Warhammer 40K</t>
+  </si>
+  <si>
+    <t>D:/My Files/My Personal Stuff/Wedding</t>
   </si>
 </sst>
 </file>
@@ -434,16 +434,16 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -451,7 +451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -459,7 +459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -467,32 +467,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
-Updated local file list spreadsheet. -Updated readme.
</commit_message>
<xml_diff>
--- a/LocalFileList.xlsx
+++ b/LocalFileList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\ROneDrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15488D5B-778C-42BE-8E59-636932B2A17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B402EE-D2D0-46D0-968E-3E62C8448F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8A96415-ACA3-4E3A-B8C9-9338A28545D5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8A96415-ACA3-4E3A-B8C9-9338A28545D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>FilesIn</t>
-  </si>
-  <si>
-    <t>AllFiles</t>
   </si>
   <si>
     <t>Path</t>
@@ -434,7 +431,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,23 +442,20 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -469,32 +463,32 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated error handling. Now the script will attempt to continue if there was an error uploading. It also outputs the number of failed uploads at the end.
</commit_message>
<xml_diff>
--- a/LocalFileList.xlsx
+++ b/LocalFileList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\ROneDrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B402EE-D2D0-46D0-968E-3E62C8448F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C40CDCD-9224-4EF9-A606-D2622DC536A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8A96415-ACA3-4E3A-B8C9-9338A28545D5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>FilesIn</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>D:/My Files/My Personal Stuff/Wedding</t>
+  </si>
+  <si>
+    <t>D:/My Files/My Personal Stuff/Documents</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DAC5BE-9D5B-4BAC-A53E-9421ABC0DC8A}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,6 +494,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>